<commit_message>
Added new file - pls check
</commit_message>
<xml_diff>
--- a/DB_Plan.xlsx
+++ b/DB_Plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dropbox\Dinmind-Support\Other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dropbox\Schneider-Ekanban-v2\Others\Git\CBDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897BACD7-1010-4C63-BAF5-BAFBE146D992}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE97F1A6-D547-455C-AF41-FBAC011806A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{48CCE496-749D-49F0-91FD-43484BA8E8C8}"/>
   </bookViews>
@@ -133,7 +133,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,8 +149,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,6 +167,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -176,10 +189,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,7 +511,7 @@
   <dimension ref="A1:A57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -516,47 +530,47 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>